<commit_message>
Update dataset and reimplement Category Trend Chart
- Updated source Excel files with January data.
- Regenerated `p2p_data.parquet`.
- Implemented robust `MainCategory` mapping in `app.py`.
- Refactored "Category-wise Spend Trend" chart to use strict aggregation:
  - One line per Main Category (e.g., Marketing, Capex).
  - No sub-category splitting.
  - Defaults to Top 5 categories.
  - Matches "Entity Trend" visual style.
- Fixed `ImportError` crash with defensive loading.

Co-authored-by: Pauriktrivedi <96005961+Pauriktrivedi@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/MLPL.xlsx
+++ b/MLPL.xlsx
@@ -245,7 +245,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">25-12-2025 06:08:28
+            <t xml:space="preserve">30-01-2026 11:08:18
 </t>
           </r>
           <r>
@@ -294,7 +294,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">25-12-2025</t>
+            <t xml:space="preserve">30-01-2026</t>
           </r>
         </is>
       </c>

</xml_diff>